<commit_message>
change test cases for saienko
</commit_message>
<xml_diff>
--- a/Template_test_cases_saienko.xlsx
+++ b/Template_test_cases_saienko.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N7\Desktop\SkillUp\skillup1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3150FD24-3ED2-4B3C-9F91-AE7E92519F7C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="312" windowWidth="15132" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="15135" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="21" r:id="rId1"/>
@@ -22,12 +28,12 @@
     <definedName name="Citing_Articles">'[3]General Search'!$B$9:$B$14</definedName>
     <definedName name="Results">'[4]General Search'!$B$9:$B$14</definedName>
   </definedNames>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <r>
       <t>How the tree directory is structured in Quality Center</t>
@@ -100,9 +106,6 @@
     </r>
   </si>
   <si>
-    <t>Search</t>
-  </si>
-  <si>
     <t>Test Case ID</t>
   </si>
   <si>
@@ -168,43 +171,139 @@
     <t>Automated (Y/N)</t>
   </si>
   <si>
-    <t>INC_CCR_PV_Premium_179</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
-    <t>Basic dataset is chosen. Create a Custom Report page is opened.</t>
-  </si>
-  <si>
-    <t>Grant Numbers Navigational counts verification.</t>
-  </si>
-  <si>
-    <t>Activate Grant Numbers limit section</t>
-  </si>
-  <si>
-    <t>Grant Numbers section opens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that  "Items 1 to 500 of ..." Navigation counts are displayed </t>
-  </si>
-  <si>
-    <t>Country Ranking report is created.</t>
-  </si>
-  <si>
-    <t>Type any valid number in "Go to item:" field and click to Go button</t>
-  </si>
-  <si>
-    <t>Navigational counts (X to Y of Z) are updated accordingly</t>
-  </si>
-  <si>
     <t>INCI-2102</t>
+  </si>
+  <si>
+    <t>Opening</t>
+  </si>
+  <si>
+    <t>Create empty file</t>
+  </si>
+  <si>
+    <t>Double-click on empty file</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>File is opened</t>
+  </si>
+  <si>
+    <t>Checking empty file can be opened</t>
+  </si>
+  <si>
+    <t>Checking filled with data file can be opened</t>
+  </si>
+  <si>
+    <t>Double-click on file</t>
+  </si>
+  <si>
+    <t>File with "qwery123" saved</t>
+  </si>
+  <si>
+    <t>File with "qwerty123"  is shown</t>
+  </si>
+  <si>
+    <t>Saving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking data can be saved </t>
+  </si>
+  <si>
+    <t>Open empty file</t>
+  </si>
+  <si>
+    <t>Type any random data</t>
+  </si>
+  <si>
+    <t>Click on Save icon</t>
+  </si>
+  <si>
+    <t>qwerty123</t>
+  </si>
+  <si>
+    <t>File saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saving </t>
+  </si>
+  <si>
+    <t>Checkin data can be saved as (with name editing etc.)</t>
+  </si>
+  <si>
+    <t>Click on "Save As" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">File saved with specified name </t>
+  </si>
+  <si>
+    <t>Page Parameters</t>
+  </si>
+  <si>
+    <t>Fill with some random text</t>
+  </si>
+  <si>
+    <t>Open "Page parameters" in "File" popup</t>
+  </si>
+  <si>
+    <t>Checking page parameters can opened</t>
+  </si>
+  <si>
+    <t>Page parameters openes correctly</t>
+  </si>
+  <si>
+    <t>Empy file created, Page parameters opened</t>
+  </si>
+  <si>
+    <t>Checking orientation can be changed</t>
+  </si>
+  <si>
+    <t>Choose landscape orientation</t>
+  </si>
+  <si>
+    <t>Choose portrait orientation</t>
+  </si>
+  <si>
+    <t>Orientation displayed correctly</t>
+  </si>
+  <si>
+    <t>Checking page size can be changed</t>
+  </si>
+  <si>
+    <t>Fill page with some random text</t>
+  </si>
+  <si>
+    <t>Fill page with some random text, open page parameters</t>
+  </si>
+  <si>
+    <t>Open page parameters</t>
+  </si>
+  <si>
+    <t>Choose difetent page sizes</t>
+  </si>
+  <si>
+    <t>Page size changes and displays correctly</t>
+  </si>
+  <si>
+    <t>Checking "fields (mm)" can be changed and displayed correctly</t>
+  </si>
+  <si>
+    <t>Fill page with random text, open page parameters</t>
+  </si>
+  <si>
+    <t>Input different parameters in fields in mm (left, right, upper, lower)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -272,7 +371,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -295,6 +394,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -314,7 +453,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -325,13 +464,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -374,43 +506,104 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Hyperlink 3" xfId="1"/>
-    <cellStyle name="Hyperlink 4" xfId="2"/>
-    <cellStyle name="Normal 2 18" xfId="3"/>
-    <cellStyle name="Normal 4 3" xfId="4"/>
-    <cellStyle name="Normal 8 3" xfId="5"/>
-    <cellStyle name="Normal 8 4" xfId="6"/>
-    <cellStyle name="Normal 8 5" xfId="7"/>
-    <cellStyle name="Normal 8 6" xfId="8"/>
-    <cellStyle name="Normal_webofscience checklist" xfId="9"/>
+    <cellStyle name="Hyperlink 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Hyperlink 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2 18" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 8 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 8 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 8 5" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 8 6" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal_webofscience checklist" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
@@ -768,7 +961,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -842,7 +1035,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -916,7 +1109,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -966,7 +1159,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -1058,7 +1251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1090,9 +1283,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1124,6 +1335,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1299,133 +1528,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="106.6640625" customWidth="1"/>
+    <col min="1" max="1" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="25"/>
+      <c r="A2" s="19"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="25"/>
+      <c r="A3" s="19"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="25"/>
+      <c r="A4" s="19"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="25"/>
+      <c r="A5" s="19"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="25"/>
+      <c r="A6" s="19"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="25"/>
+      <c r="A7" s="19"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="19"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="19"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="19"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="19"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="19"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="19"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="19"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="19"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="19"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="19"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="25"/>
+      <c r="A18" s="19"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="25"/>
+      <c r="A19" s="19"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="25"/>
+      <c r="A20" s="19"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="25"/>
+      <c r="A21" s="19"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="25"/>
+      <c r="A22" s="19"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="25"/>
+      <c r="A23" s="19"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="25"/>
+      <c r="A24" s="19"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="25"/>
+      <c r="A25" s="19"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="25"/>
+      <c r="A26" s="19"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="25"/>
+      <c r="A27" s="19"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="25"/>
+      <c r="A28" s="19"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="25"/>
+      <c r="A29" s="19"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="25"/>
+      <c r="A30" s="19"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="25"/>
+      <c r="A31" s="19"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="25"/>
+      <c r="A32" s="19"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="25"/>
+      <c r="A33" s="19"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="25"/>
+      <c r="A34" s="19"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="25"/>
+      <c r="A35" s="19"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="25"/>
+      <c r="A36" s="19"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="25"/>
+      <c r="A37" s="19"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="25"/>
+      <c r="A38" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1438,370 +1667,653 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="10"/>
-    <col min="3" max="3" width="9.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="33.44140625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="11"/>
-    <col min="7" max="7" width="62" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="63.5546875" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="10"/>
+    <col min="1" max="2" width="9.140625" style="8"/>
+    <col min="3" max="3" width="9.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="62" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="63.5703125" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="12" customFormat="1" ht="66">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="63.75">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:19" s="10" customFormat="1">
+      <c r="A2" s="35">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="52.8">
-      <c r="A2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="4"/>
       <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="7"/>
-    </row>
-    <row r="3" spans="1:19" s="12" customFormat="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="25.5">
+      <c r="A3" s="35">
+        <v>2</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="25.5">
+      <c r="A4" s="33">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" s="10" customFormat="1">
+      <c r="A5" s="34"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="7"/>
-    </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="26.4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3">
+      <c r="G5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="37"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="12"/>
+    </row>
+    <row r="6" spans="1:19" s="10" customFormat="1">
+      <c r="A6" s="34"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="3">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="1:19" s="12" customFormat="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="14"/>
-    </row>
-    <row r="6" spans="1:19" s="12" customFormat="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="14"/>
-    </row>
-    <row r="7" spans="1:19" s="12" customFormat="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="14"/>
-    </row>
-    <row r="8" spans="1:19" s="12" customFormat="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="14"/>
-    </row>
-    <row r="9" spans="1:19" s="12" customFormat="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="14"/>
-    </row>
-    <row r="10" spans="1:19" s="12" customFormat="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="14"/>
-    </row>
-    <row r="11" spans="1:19" s="12" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="14"/>
-    </row>
-    <row r="12" spans="1:19" s="12" customFormat="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="14"/>
-    </row>
-    <row r="13" spans="1:19" s="12" customFormat="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="14"/>
+      <c r="G6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="37"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="12"/>
+    </row>
+    <row r="7" spans="1:19" s="10" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A7" s="34">
+        <v>4</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="16">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="12"/>
+    </row>
+    <row r="8" spans="1:19" s="10" customFormat="1">
+      <c r="A8" s="34"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="16">
+        <v>2</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="37"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="12"/>
+    </row>
+    <row r="9" spans="1:19" s="10" customFormat="1">
+      <c r="A9" s="34"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="16">
+        <v>3</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="37"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="12"/>
+    </row>
+    <row r="10" spans="1:19" s="10" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A10" s="34">
+        <v>5</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="12"/>
+    </row>
+    <row r="11" spans="1:19" s="10" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A11" s="34"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="16">
+        <v>2</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="37"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="12"/>
+    </row>
+    <row r="12" spans="1:19" s="10" customFormat="1">
+      <c r="A12" s="34"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="16">
+        <v>3</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="37"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="12"/>
+    </row>
+    <row r="13" spans="1:19" s="10" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A13" s="34">
+        <v>6</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="12"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="34"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="9">
+        <v>2</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="37"/>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="34"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="9">
+        <v>3</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="37"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:19" ht="38.25" customHeight="1">
+      <c r="A16" s="41">
+        <v>7</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="41"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="9">
+        <v>2</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="42"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="41"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="9">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="42"/>
+    </row>
+    <row r="19" spans="1:9" ht="38.25" customHeight="1">
+      <c r="A19" s="41">
+        <v>8</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="41"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="9">
+        <v>2</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="40"/>
+      <c r="I20" s="42"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I4 G4:G6 I12:I13 G12:G13">
+  <mergeCells count="42">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I4 G4:G6 I13 G12:G13">
     <cfRule type="cellIs" priority="79" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
@@ -1812,7 +2324,7 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 G4:G6 I12:I13 G12:G13">
+  <conditionalFormatting sqref="I4 G4:G6 I13 G12:G13">
     <cfRule type="cellIs" priority="76" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
@@ -1889,50 +2401,6 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="40" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="41" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="42" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="38" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="39" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="34" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="35" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="36" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="32" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="33" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I4">
     <cfRule type="cellIs" priority="28" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
@@ -1977,40 +2445,18 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" priority="16" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="17" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="G7:I7 G10:I10 G8:G9 G11">
+    <cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="14" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="15" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:I11">
-    <cfRule type="cellIs" priority="4" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:I11">
+  <conditionalFormatting sqref="G7:I7 G10:I10 G8:G9 G11">
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>

</xml_diff>